<commit_message>
Changed key response values
</commit_message>
<xml_diff>
--- a/random.xlsx
+++ b/random.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="1580" windowWidth="24480" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="680" yWindow="0" windowWidth="24480" windowHeight="16600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>randomPaw</t>
   </si>
@@ -36,18 +36,9 @@
     <t>['1']</t>
   </si>
   <si>
-    <t>['2']</t>
-  </si>
-  <si>
-    <t>['3']</t>
-  </si>
-  <si>
     <t>['4']</t>
   </si>
   <si>
-    <t>['2', '1', '3','4']</t>
-  </si>
-  <si>
     <t>correctKey</t>
   </si>
   <si>
@@ -61,6 +52,18 @@
   </si>
   <si>
     <t>min4.png</t>
+  </si>
+  <si>
+    <t>correctKeyPress</t>
+  </si>
+  <si>
+    <t>['7']</t>
+  </si>
+  <si>
+    <t>['0']</t>
+  </si>
+  <si>
+    <t>['7', '4', '1','0']</t>
   </si>
 </sst>
 </file>
@@ -73,7 +76,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -112,8 +114,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -168,7 +172,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -192,6 +196,7 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -215,6 +220,7 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,29 +569,35 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -593,33 +605,42 @@
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>